<commit_message>
Update result reference to FRObservationResultDocument cefe7315bd46cc99e35cf705ab3ea5f65dc03f3b
</commit_message>
<xml_diff>
--- a/BrancheIntermediare/ig/StructureDefinition-fr-diagnostic-report-imaging-document.xlsx
+++ b/BrancheIntermediare/ig/StructureDefinition-fr-diagnostic-report-imaging-document.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T16:46:30+00:00</t>
+    <t>2025-12-03T16:47:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1213,7 +1213,7 @@
 Atomic ValueResultAtomic resultDataTestAnalyteBatteryOrganizer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Observation|4.0.1)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/fr-observation-result-document)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
MAJ des profils spécifiques à l'magerie (#75)
* MAJ des profils d'imagerie suite aux remarques de Alain

* Corrections commentaires b00fceebf9aa6e68bd4bd879bb631e4886606801
</commit_message>
<xml_diff>
--- a/BrancheIntermediare/ig/StructureDefinition-fr-diagnostic-report-imaging-document.xlsx
+++ b/BrancheIntermediare/ig/StructureDefinition-fr-diagnostic-report-imaging-document.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="445">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-04T14:08:40+00:00</t>
+    <t>2025-12-05T10:50:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -507,19 +507,6 @@
   </si>
   <si>
     <t>Imaging procedure used for the imaging acquisition</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.extension:informationDuPatient</t>
-  </si>
-  <si>
-    <t>informationDuPatient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/fr-education-patient-extension}
-</t>
-  </si>
-  <si>
-    <t>Informations du patient</t>
   </si>
   <si>
     <t>DiagnosticReport.modifierExtension</t>
@@ -1217,22 +1204,51 @@
 </t>
   </si>
   <si>
-    <t>Résultats de l'acte d'imagerie</t>
+    <t>Résultats d'examen (actuels ou antérieurs)</t>
   </si>
   <si>
     <t>[Observations](http://hl7.org/fhir/R4/observation.html)  that are part of this diagnostic report.</t>
   </si>
   <si>
+    <t>Les résultats sont exprimés sous forme non codée dans notre cas d’usage. Le contenu narratif du résultat est porté dans une note</t>
+  </si>
+  <si>
+    <t>Need to support individual results, or  groups of results, where the result grouping is arbitrary, but meaningful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pattern:reference}
+</t>
+  </si>
+  <si>
+    <t>OBXs</t>
+  </si>
+  <si>
+    <t>outboundRelationship[typeCode=COMP].target</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.result:resultatActuel</t>
+  </si>
+  <si>
+    <t>resultatActuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Observation|4.0.1)
+</t>
+  </si>
+  <si>
+    <t>Résultats actuels de l'examen d'imagerie</t>
+  </si>
+  <si>
     <t>Observations can contain observations.</t>
   </si>
   <si>
-    <t>Need to support individual results, or  groups of results, where the result grouping is arbitrary, but meaningful.</t>
-  </si>
-  <si>
-    <t>OBXs</t>
-  </si>
-  <si>
-    <t>outboundRelationship[typeCode=COMP].target</t>
+    <t>DiagnosticReport.result:resultatAnterieur</t>
+  </si>
+  <si>
+    <t>resultatAnterieur</t>
+  </si>
+  <si>
+    <t>Résultats antérieurs</t>
   </si>
   <si>
     <t>DiagnosticReport.imagingStudy</t>
@@ -1365,7 +1381,7 @@
     <t>DiagnosticReport.conclusionCode</t>
   </si>
   <si>
-    <t>Conclusions codées du rapport d’imagerie.</t>
+    <t>Codes for the clinical conclusion of test results</t>
   </si>
   <si>
     <t>One or more codes that represent the summary conclusion (interpretation/impression) of the diagnostic report.</t>
@@ -1719,7 +1735,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN65"/>
+  <dimension ref="A1:AN66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3139,18 +3155,16 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>157</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="C13" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>80</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
@@ -3160,25 +3174,29 @@
         <v>79</v>
       </c>
       <c r="H13" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I13" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="I13" t="s" s="2">
-        <v>80</v>
-      </c>
       <c r="J13" t="s" s="2">
         <v>80</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>159</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>160</v>
       </c>
       <c r="M13" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="N13" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="O13" t="s" s="2">
+        <v>162</v>
+      </c>
       <c r="P13" t="s" s="2">
         <v>80</v>
       </c>
@@ -3226,7 +3244,7 @@
         <v>80</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>78</v>
@@ -3235,7 +3253,7 @@
         <v>79</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>141</v>
@@ -3247,7 +3265,7 @@
         <v>80</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>80</v>
@@ -3255,18 +3273,18 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>79</v>
@@ -3275,25 +3293,25 @@
         <v>80</v>
       </c>
       <c r="I14" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J14" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="J14" t="s" s="2">
-        <v>80</v>
-      </c>
       <c r="K14" t="s" s="2">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>80</v>
@@ -3342,7 +3360,7 @@
         <v>80</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>78</v>
@@ -3354,62 +3372,62 @@
         <v>80</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>80</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>79</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>80</v>
@@ -3446,19 +3464,17 @@
         <v>80</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="AC15" s="2"/>
       <c r="AD15" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>78</v>
@@ -3473,28 +3489,30 @@
         <v>102</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>178</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>187</v>
+      </c>
       <c r="D16" t="s" s="2">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3504,7 +3522,7 @@
         <v>79</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>80</v>
@@ -3513,19 +3531,19 @@
         <v>80</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="L16" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="N16" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="O16" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="O16" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>80</v>
@@ -3562,17 +3580,19 @@
         <v>80</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AC16" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="AD16" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>78</v>
@@ -3587,13 +3607,13 @@
         <v>102</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AN16" t="s" s="2">
         <v>80</v>
@@ -3604,44 +3624,40 @@
         <v>190</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="C17" t="s" s="2">
-        <v>191</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="L17" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="M17" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="N17" s="2"/>
+      <c r="O17" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>80</v>
@@ -3666,13 +3682,13 @@
         <v>80</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>80</v>
+        <v>194</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>80</v>
+        <v>195</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>80</v>
@@ -3690,13 +3706,13 @@
         <v>80</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>80</v>
@@ -3705,58 +3721,58 @@
         <v>102</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>80</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s" s="2">
         <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>110</v>
+        <v>202</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N18" s="2"/>
-      <c r="O18" t="s" s="2">
-        <v>197</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="N18" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
         <v>80</v>
       </c>
@@ -3780,13 +3796,13 @@
         <v>80</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>80</v>
@@ -3804,13 +3820,13 @@
         <v>80</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>80</v>
@@ -3819,35 +3835,35 @@
         <v>102</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>80</v>
@@ -3859,17 +3875,15 @@
         <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>209</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
         <v>80</v>
@@ -3894,37 +3908,35 @@
         <v>80</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="Y19" t="s" s="2">
-        <v>211</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="Y19" s="2"/>
       <c r="Z19" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AA19" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE19" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF19" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="AA19" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB19" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC19" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD19" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE19" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AF19" t="s" s="2">
-        <v>204</v>
-      </c>
       <c r="AG19" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>80</v>
@@ -3933,32 +3945,32 @@
         <v>102</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>80</v>
+        <v>217</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>90</v>
@@ -3973,16 +3985,18 @@
         <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
+      <c r="O20" t="s" s="2">
+        <v>226</v>
+      </c>
       <c r="P20" t="s" s="2">
         <v>80</v>
       </c>
@@ -4006,11 +4020,13 @@
         <v>80</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="Y20" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="Y20" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="Z20" t="s" s="2">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>80</v>
@@ -4028,10 +4044,10 @@
         <v>80</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>90</v>
@@ -4043,28 +4059,28 @@
         <v>102</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -4083,17 +4099,19 @@
         <v>91</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="O21" t="s" s="2">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>80</v>
@@ -4142,7 +4160,7 @@
         <v>80</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -4157,28 +4175,28 @@
         <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
@@ -4197,19 +4215,19 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>80</v>
@@ -4258,7 +4276,7 @@
         <v>80</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4273,28 +4291,28 @@
         <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -4313,19 +4331,19 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>80</v>
@@ -4374,7 +4392,7 @@
         <v>80</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4389,38 +4407,38 @@
         <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>253</v>
+        <v>80</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>80</v>
@@ -4429,19 +4447,19 @@
         <v>91</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>80</v>
@@ -4478,25 +4496,23 @@
         <v>80</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC24" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="AC24" s="2"/>
       <c r="AD24" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>80</v>
@@ -4505,28 +4521,30 @@
         <v>102</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>80</v>
+        <v>270</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>275</v>
+      </c>
       <c r="D25" t="s" s="2">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4536,7 +4554,7 @@
         <v>79</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>80</v>
@@ -4545,19 +4563,19 @@
         <v>91</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="O25" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="O25" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>80</v>
@@ -4594,17 +4612,19 @@
         <v>80</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AC25" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="AC25" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="AD25" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4619,30 +4639,28 @@
         <v>102</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
         <v>278</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="C26" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="D26" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4652,7 +4670,7 @@
         <v>79</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>80</v>
@@ -4661,19 +4679,19 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="M26" t="s" s="2">
-        <v>271</v>
-      </c>
       <c r="N26" t="s" s="2">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>80</v>
@@ -4722,7 +4740,7 @@
         <v>80</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4737,60 +4755,56 @@
         <v>102</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>283</v>
+        <v>80</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>273</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>80</v>
       </c>
@@ -4838,39 +4852,39 @@
         <v>80</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>274</v>
+        <v>80</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>287</v>
+        <v>80</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>277</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4878,10 +4892,10 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>80</v>
@@ -4893,13 +4907,13 @@
         <v>80</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4938,16 +4952,16 @@
         <v>80</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="AD28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>292</v>
@@ -4956,13 +4970,13 @@
         <v>78</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>80</v>
@@ -4971,7 +4985,7 @@
         <v>80</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>80</v>
@@ -4979,12 +4993,14 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="C29" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="B29" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
         <v>80</v>
       </c>
@@ -5005,13 +5021,13 @@
         <v>80</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>135</v>
+        <v>295</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>136</v>
+        <v>296</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>137</v>
+        <v>297</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5050,19 +5066,19 @@
         <v>80</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="AC29" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AD29" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5091,24 +5107,22 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="C30" t="s" s="2">
-        <v>298</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G30" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="G30" t="s" s="2">
-        <v>79</v>
-      </c>
       <c r="H30" t="s" s="2">
         <v>80</v>
       </c>
@@ -5119,13 +5133,13 @@
         <v>80</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5176,19 +5190,19 @@
         <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>80</v>
@@ -5197,7 +5211,7 @@
         <v>80</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>80</v>
@@ -5205,10 +5219,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5216,10 +5230,10 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>78</v>
+        <v>302</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>80</v>
@@ -5231,13 +5245,13 @@
         <v>80</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5276,16 +5290,16 @@
         <v>80</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="AD31" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>292</v>
@@ -5294,13 +5308,13 @@
         <v>78</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>80</v>
@@ -5309,7 +5323,7 @@
         <v>80</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>80</v>
@@ -5317,21 +5331,23 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="C32" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="B32" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
-        <v>306</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>80</v>
@@ -5388,19 +5404,19 @@
         <v>80</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="AC32" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AD32" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5429,20 +5445,18 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>308</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>90</v>
@@ -5457,13 +5471,13 @@
         <v>80</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>136</v>
+        <v>286</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>137</v>
+        <v>287</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5514,19 +5528,19 @@
         <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>80</v>
@@ -5535,7 +5549,7 @@
         <v>80</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>80</v>
@@ -5543,10 +5557,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5557,7 +5571,7 @@
         <v>78</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>80</v>
@@ -5569,13 +5583,13 @@
         <v>80</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5614,16 +5628,16 @@
         <v>80</v>
       </c>
       <c r="AB34" t="s" s="2">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="AC34" t="s" s="2">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="AD34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>292</v>
@@ -5632,13 +5646,13 @@
         <v>78</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>80</v>
@@ -5647,7 +5661,7 @@
         <v>80</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>80</v>
@@ -5655,10 +5669,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5666,10 +5680,10 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>80</v>
@@ -5681,22 +5695,24 @@
         <v>80</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>136</v>
+        <v>311</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" t="s" s="2">
-        <v>80</v>
+        <v>304</v>
       </c>
       <c r="S35" t="s" s="2">
         <v>80</v>
@@ -5726,31 +5742,31 @@
         <v>80</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="AC35" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AD35" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>80</v>
@@ -5759,7 +5775,7 @@
         <v>80</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>80</v>
@@ -5767,10 +5783,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5778,7 +5794,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>90</v>
@@ -5793,27 +5809,25 @@
         <v>80</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" t="s" s="2">
-        <v>308</v>
+        <v>80</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>80</v>
+        <v>319</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>80</v>
@@ -5828,13 +5842,11 @@
         <v>80</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y36" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="Y36" s="2"/>
       <c r="Z36" t="s" s="2">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>80</v>
@@ -5852,10 +5864,10 @@
         <v>80</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>90</v>
@@ -5864,7 +5876,7 @@
         <v>80</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>80</v>
@@ -5881,12 +5893,14 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>323</v>
+      </c>
       <c r="D37" t="s" s="2">
         <v>80</v>
       </c>
@@ -5907,13 +5921,13 @@
         <v>80</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>322</v>
+        <v>137</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5925,7 +5939,7 @@
         <v>80</v>
       </c>
       <c r="S37" t="s" s="2">
-        <v>323</v>
+        <v>80</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>80</v>
@@ -5940,11 +5954,13 @@
         <v>80</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="Y37" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="Z37" t="s" s="2">
-        <v>324</v>
+        <v>80</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>80</v>
@@ -5962,19 +5978,19 @@
         <v>80</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>325</v>
+        <v>292</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>80</v>
@@ -5983,7 +5999,7 @@
         <v>80</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>80</v>
@@ -5991,14 +6007,12 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>327</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
         <v>80</v>
       </c>
@@ -6019,13 +6033,13 @@
         <v>80</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>328</v>
+        <v>286</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>137</v>
+        <v>287</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6076,19 +6090,19 @@
         <v>80</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>80</v>
@@ -6097,7 +6111,7 @@
         <v>80</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>80</v>
@@ -6105,10 +6119,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6119,7 +6133,7 @@
         <v>78</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>80</v>
@@ -6131,13 +6145,13 @@
         <v>80</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6176,16 +6190,16 @@
         <v>80</v>
       </c>
       <c r="AB39" t="s" s="2">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="AC39" t="s" s="2">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="AD39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>292</v>
@@ -6194,13 +6208,13 @@
         <v>78</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>80</v>
@@ -6209,7 +6223,7 @@
         <v>80</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>80</v>
@@ -6217,10 +6231,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6228,10 +6242,10 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>80</v>
@@ -6243,22 +6257,24 @@
         <v>80</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>136</v>
+        <v>311</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N40" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" t="s" s="2">
-        <v>80</v>
+        <v>323</v>
       </c>
       <c r="S40" t="s" s="2">
         <v>80</v>
@@ -6288,31 +6304,31 @@
         <v>80</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="AC40" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AD40" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>80</v>
@@ -6321,7 +6337,7 @@
         <v>80</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>80</v>
@@ -6329,10 +6345,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6340,7 +6356,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>90</v>
@@ -6355,24 +6371,22 @@
         <v>80</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" t="s" s="2">
-        <v>327</v>
+        <v>80</v>
       </c>
       <c r="S41" t="s" s="2">
         <v>80</v>
@@ -6414,10 +6428,10 @@
         <v>80</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>90</v>
@@ -6426,7 +6440,7 @@
         <v>80</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>80</v>
@@ -6443,18 +6457,20 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="D42" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>90</v>
@@ -6469,13 +6485,13 @@
         <v>80</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>321</v>
+        <v>136</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>322</v>
+        <v>137</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6526,19 +6542,19 @@
         <v>80</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>325</v>
+        <v>292</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>80</v>
@@ -6547,7 +6563,7 @@
         <v>80</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>80</v>
@@ -6555,20 +6571,18 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>334</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>90</v>
@@ -6583,13 +6597,13 @@
         <v>80</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>136</v>
+        <v>286</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>137</v>
+        <v>287</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6640,19 +6654,19 @@
         <v>80</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>80</v>
@@ -6661,7 +6675,7 @@
         <v>80</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>80</v>
@@ -6669,10 +6683,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6683,7 +6697,7 @@
         <v>78</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>80</v>
@@ -6695,13 +6709,13 @@
         <v>80</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6740,16 +6754,16 @@
         <v>80</v>
       </c>
       <c r="AB44" t="s" s="2">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="AC44" t="s" s="2">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="AD44" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>292</v>
@@ -6758,13 +6772,13 @@
         <v>78</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>80</v>
@@ -6773,7 +6787,7 @@
         <v>80</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>80</v>
@@ -6781,10 +6795,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6792,10 +6806,10 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>80</v>
@@ -6807,22 +6821,24 @@
         <v>80</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>136</v>
+        <v>311</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" t="s" s="2">
-        <v>80</v>
+        <v>330</v>
       </c>
       <c r="S45" t="s" s="2">
         <v>80</v>
@@ -6852,31 +6868,31 @@
         <v>80</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="AC45" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AD45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>80</v>
@@ -6885,7 +6901,7 @@
         <v>80</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>80</v>
@@ -6893,10 +6909,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6904,7 +6920,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>90</v>
@@ -6919,24 +6935,22 @@
         <v>80</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>104</v>
+        <v>335</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" t="s" s="2">
-        <v>334</v>
+        <v>80</v>
       </c>
       <c r="S46" t="s" s="2">
         <v>80</v>
@@ -6978,10 +6992,10 @@
         <v>80</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>90</v>
@@ -6990,7 +7004,7 @@
         <v>80</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>80</v>
@@ -7007,10 +7021,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7018,7 +7032,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>90</v>
@@ -7033,22 +7047,24 @@
         <v>80</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>339</v>
+        <v>104</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N47" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" t="s" s="2">
-        <v>80</v>
+        <v>338</v>
       </c>
       <c r="S47" t="s" s="2">
         <v>80</v>
@@ -7090,10 +7106,10 @@
         <v>80</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>90</v>
@@ -7102,7 +7118,7 @@
         <v>80</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>80</v>
@@ -7119,10 +7135,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="B48" t="s" s="2">
         <v>340</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7130,10 +7146,10 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>80</v>
@@ -7145,24 +7161,22 @@
         <v>80</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>104</v>
+        <v>341</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" t="s" s="2">
-        <v>342</v>
+        <v>80</v>
       </c>
       <c r="S48" t="s" s="2">
         <v>80</v>
@@ -7204,10 +7218,10 @@
         <v>80</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>90</v>
@@ -7216,7 +7230,7 @@
         <v>80</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>80</v>
@@ -7233,10 +7247,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7247,7 +7261,7 @@
         <v>78</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>80</v>
@@ -7256,18 +7270,20 @@
         <v>80</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="N49" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
         <v>80</v>
@@ -7316,7 +7332,7 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7325,7 +7341,7 @@
         <v>90</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>80</v>
+        <v>347</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>102</v>
@@ -7345,10 +7361,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7371,16 +7387,16 @@
         <v>91</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7406,13 +7422,13 @@
         <v>80</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>80</v>
+        <v>352</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>80</v>
+        <v>353</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>80</v>
+        <v>354</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>80</v>
@@ -7430,7 +7446,7 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7439,7 +7455,7 @@
         <v>90</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>351</v>
+        <v>80</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>102</v>
@@ -7459,10 +7475,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7485,16 +7501,16 @@
         <v>91</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
@@ -7520,13 +7536,13 @@
         <v>80</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>356</v>
+        <v>80</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>357</v>
+        <v>80</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>358</v>
+        <v>80</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>80</v>
@@ -7544,7 +7560,7 @@
         <v>80</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
@@ -7565,7 +7581,7 @@
         <v>80</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>133</v>
+        <v>361</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>80</v>
@@ -7573,10 +7589,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7599,16 +7615,16 @@
         <v>91</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>170</v>
+        <v>285</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7658,7 +7674,7 @@
         <v>80</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
@@ -7679,7 +7695,7 @@
         <v>80</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>365</v>
+        <v>133</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>80</v>
@@ -7687,10 +7703,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7701,7 +7717,7 @@
         <v>78</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>80</v>
@@ -7710,21 +7726,23 @@
         <v>80</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>289</v>
+        <v>368</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="O53" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>372</v>
+      </c>
       <c r="P53" t="s" s="2">
         <v>80</v>
       </c>
@@ -7772,13 +7790,13 @@
         <v>80</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>80</v>
@@ -7790,10 +7808,10 @@
         <v>80</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>80</v>
+        <v>373</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>133</v>
+        <v>229</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>80</v>
@@ -7801,14 +7819,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>80</v>
+        <v>375</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -7818,7 +7836,7 @@
         <v>79</v>
       </c>
       <c r="H54" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I54" t="s" s="2">
         <v>80</v>
@@ -7827,19 +7845,19 @@
         <v>80</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="O54" t="s" s="2">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>80</v>
@@ -7876,19 +7894,17 @@
         <v>80</v>
       </c>
       <c r="AB54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="AC54" s="2"/>
       <c r="AD54" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>78</v>
@@ -7906,35 +7922,37 @@
         <v>80</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>233</v>
+        <v>383</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="C55" s="2"/>
+        <v>374</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>385</v>
+      </c>
       <c r="D55" t="s" s="2">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>80</v>
@@ -7943,19 +7961,19 @@
         <v>80</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="O55" t="s" s="2">
         <v>380</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>80</v>
@@ -8004,7 +8022,7 @@
         <v>80</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
@@ -8022,10 +8040,10 @@
         <v>80</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>80</v>
@@ -8033,21 +8051,23 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>374</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>390</v>
+      </c>
       <c r="D56" t="s" s="2">
-        <v>80</v>
+        <v>375</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>80</v>
@@ -8059,18 +8079,20 @@
         <v>80</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="N56" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L56" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="O56" s="2"/>
+      <c r="O56" t="s" s="2">
+        <v>380</v>
+      </c>
       <c r="P56" t="s" s="2">
         <v>80</v>
       </c>
@@ -8118,7 +8140,7 @@
         <v>80</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>78</v>
@@ -8136,10 +8158,10 @@
         <v>80</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>80</v>
+        <v>382</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>80</v>
@@ -8147,14 +8169,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>394</v>
+        <v>80</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -8170,21 +8192,21 @@
         <v>80</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="M57" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="N57" s="2"/>
-      <c r="O57" t="s" s="2">
-        <v>398</v>
-      </c>
+      <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
         <v>80</v>
       </c>
@@ -8232,7 +8254,7 @@
         <v>80</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8250,10 +8272,10 @@
         <v>80</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>399</v>
+        <v>80</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>80</v>
@@ -8261,21 +8283,21 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>80</v>
+        <v>399</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>80</v>
@@ -8284,19 +8306,21 @@
         <v>80</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>289</v>
+        <v>400</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>290</v>
+        <v>401</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>291</v>
+        <v>402</v>
       </c>
       <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
+      <c r="O58" t="s" s="2">
+        <v>403</v>
+      </c>
       <c r="P58" t="s" s="2">
         <v>80</v>
       </c>
@@ -8344,28 +8368,28 @@
         <v>80</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>292</v>
+        <v>398</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>80</v>
+        <v>404</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>293</v>
+        <v>383</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>80</v>
@@ -8373,21 +8397,21 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
-        <v>162</v>
+        <v>80</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>80</v>
@@ -8399,17 +8423,15 @@
         <v>80</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>402</v>
+        <v>286</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>80</v>
@@ -8458,19 +8480,19 @@
         <v>80</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>80</v>
@@ -8479,7 +8501,7 @@
         <v>80</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>80</v>
@@ -8487,14 +8509,14 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
-        <v>405</v>
+        <v>158</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
@@ -8507,26 +8529,24 @@
         <v>80</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K60" t="s" s="2">
         <v>135</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="O60" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>80</v>
       </c>
@@ -8574,7 +8594,7 @@
         <v>80</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>408</v>
+        <v>292</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>78</v>
@@ -8595,7 +8615,7 @@
         <v>80</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>133</v>
+        <v>289</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>80</v>
@@ -8610,38 +8630,38 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>289</v>
+        <v>135</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>412</v>
+        <v>161</v>
       </c>
       <c r="O61" t="s" s="2">
-        <v>413</v>
+        <v>162</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>80</v>
@@ -8690,19 +8710,19 @@
         <v>80</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>80</v>
@@ -8711,7 +8731,7 @@
         <v>80</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>414</v>
+        <v>133</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>80</v>
@@ -8719,10 +8739,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8730,7 +8750,7 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>90</v>
@@ -8742,19 +8762,23 @@
         <v>80</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="O62" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>80</v>
       </c>
@@ -8802,10 +8826,10 @@
         <v>80</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>90</v>
@@ -8829,7 +8853,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
         <v>420</v>
       </c>
@@ -8838,26 +8862,26 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>421</v>
+        <v>80</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>90</v>
       </c>
       <c r="H63" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I63" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J63" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="I63" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="J63" t="s" s="2">
-        <v>80</v>
-      </c>
       <c r="K63" t="s" s="2">
-        <v>289</v>
+        <v>421</v>
       </c>
       <c r="L63" t="s" s="2">
         <v>422</v>
@@ -8866,9 +8890,7 @@
         <v>423</v>
       </c>
       <c r="N63" s="2"/>
-      <c r="O63" t="s" s="2">
-        <v>424</v>
-      </c>
+      <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
         <v>80</v>
       </c>
@@ -8919,7 +8941,7 @@
         <v>420</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>90</v>
@@ -8934,10 +8956,10 @@
         <v>80</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>425</v>
+        <v>80</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>80</v>
@@ -8945,21 +8967,21 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>80</v>
+        <v>426</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>91</v>
@@ -8971,16 +8993,18 @@
         <v>80</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>206</v>
+        <v>285</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="N64" s="2"/>
+      <c r="O64" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
         <v>80</v>
       </c>
@@ -9004,13 +9028,13 @@
         <v>80</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>210</v>
+        <v>80</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>430</v>
+        <v>80</v>
       </c>
       <c r="Z64" t="s" s="2">
-        <v>431</v>
+        <v>80</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>80</v>
@@ -9028,13 +9052,13 @@
         <v>80</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>80</v>
@@ -9046,10 +9070,10 @@
         <v>80</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>80</v>
@@ -9057,10 +9081,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9083,20 +9107,16 @@
         <v>80</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L65" t="s" s="2">
-        <v>435</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="O65" t="s" s="2">
-        <v>438</v>
-      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>80</v>
       </c>
@@ -9120,13 +9140,13 @@
         <v>80</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>80</v>
+        <v>206</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>80</v>
+        <v>435</v>
       </c>
       <c r="Z65" t="s" s="2">
-        <v>80</v>
+        <v>436</v>
       </c>
       <c r="AA65" t="s" s="2">
         <v>80</v>
@@ -9144,7 +9164,7 @@
         <v>80</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>78</v>
@@ -9162,17 +9182,133 @@
         <v>80</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="AM65" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="AN65" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" hidden="true">
+      <c r="A66" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="B66" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K66" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="AN65" t="s" s="2">
+      <c r="L66" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="P66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q66" s="2"/>
+      <c r="R66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AM66" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="AN66" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN65">
+  <autoFilter ref="A1:AN66">
     <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9182,7 +9318,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI64">
+  <conditionalFormatting sqref="A2:AI65">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>